<commit_message>
Updated study guide 9-24
</commit_message>
<xml_diff>
--- a/StudyGuide.xlsx
+++ b/StudyGuide.xlsx
@@ -32,8 +32,12 @@
     <sheet name="2A Core Conversations" sheetId="21" r:id="rId18"/>
     <sheet name="2A Drill B" sheetId="23" r:id="rId19"/>
     <sheet name="2A Drill C" sheetId="24" r:id="rId20"/>
-    <sheet name="2A Practice" sheetId="25" r:id="rId21"/>
-    <sheet name="Drill Template (2)" sheetId="11" r:id="rId22"/>
+    <sheet name="2A Drill E" sheetId="26" r:id="rId21"/>
+    <sheet name="2A Drill F" sheetId="27" r:id="rId22"/>
+    <sheet name="2A Drill G" sheetId="28" r:id="rId23"/>
+    <sheet name="2A Practice" sheetId="25" r:id="rId24"/>
+    <sheet name="Drill Template (3)" sheetId="30" r:id="rId25"/>
+    <sheet name="Drill Template (2)" sheetId="11" r:id="rId26"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -45,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1939" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2244" uniqueCount="792">
   <si>
     <t>Imperfective
 Negative</t>
@@ -2619,12 +2623,6 @@
     <t>You've been asked if you attended a particular exhibit yesterday. Explain that that's not correct: you are going tomorrow.</t>
   </si>
   <si>
-    <t>Iie, kinoo ikimasen desita. Asita ikimasu yo.</t>
-  </si>
-  <si>
-    <t>No, I did not go yesterday. I am going tomorrow.</t>
-  </si>
-  <si>
     <t>You've just learned that a colleague knows how to make Chinese food. Ask if he makes it often.</t>
   </si>
   <si>
@@ -2692,6 +2690,314 @@
   </si>
   <si>
     <t>Did you go yesterday? No, it's different. I am going tomorrow.</t>
+  </si>
+  <si>
+    <t>Ee, wakarimasu.</t>
+  </si>
+  <si>
+    <t>Yes, I understand.</t>
+  </si>
+  <si>
+    <t>Reply</t>
+  </si>
+  <si>
+    <t>I will play, thank you. (Accept invitation)</t>
+  </si>
+  <si>
+    <t>Iie, amari takaku nakatta desu yo.</t>
+  </si>
+  <si>
+    <t>Drill E7</t>
+  </si>
+  <si>
+    <t>Drill E8</t>
+  </si>
+  <si>
+    <t>I guess I do go often.</t>
+  </si>
+  <si>
+    <t>Denwa desita ka?</t>
+  </si>
+  <si>
+    <t>Iie, denwa zya arimasen desita yo.</t>
+  </si>
+  <si>
+    <t>Was it a phone call?</t>
+  </si>
+  <si>
+    <t>No, it was not a phone call.</t>
+  </si>
+  <si>
+    <t>Iie, dame zya arimasen desita yo.</t>
+  </si>
+  <si>
+    <t>Kiree desita ka?</t>
+  </si>
+  <si>
+    <t>Iie, kiree zya arimasen desita yo.</t>
+  </si>
+  <si>
+    <t>Was it broken?</t>
+  </si>
+  <si>
+    <t>No, it was not broken.</t>
+  </si>
+  <si>
+    <t>Was it beautiful?</t>
+  </si>
+  <si>
+    <t>No, it was not beautiful.</t>
+  </si>
+  <si>
+    <t>Eego desita ka?</t>
+  </si>
+  <si>
+    <t>Iie, eego zya arimasen desita yo.</t>
+  </si>
+  <si>
+    <t>Was it English?</t>
+  </si>
+  <si>
+    <t>No, it was not English.</t>
+  </si>
+  <si>
+    <t>Kyooto desita ka?</t>
+  </si>
+  <si>
+    <t>Iie, Kyooto zya arimasen desita yo.</t>
+  </si>
+  <si>
+    <t>Was it Kyooto?</t>
+  </si>
+  <si>
+    <t>No, it was not Kyooto.</t>
+  </si>
+  <si>
+    <t>Tanaka-san desita ka?</t>
+  </si>
+  <si>
+    <t>Iie, Tanaka-san zya arimasen desita yo.</t>
+  </si>
+  <si>
+    <t>Was it Mr. Tanaka?</t>
+  </si>
+  <si>
+    <t>No, it was not Mr. Tanaka.</t>
+  </si>
+  <si>
+    <t>Rosiago desita ka?</t>
+  </si>
+  <si>
+    <t>Iie, Rosiago zya arimasen desita yo.</t>
+  </si>
+  <si>
+    <t>Was it Russian?</t>
+  </si>
+  <si>
+    <t>No, it was not Russian.</t>
+  </si>
+  <si>
+    <t>Tegami desita ka?</t>
+  </si>
+  <si>
+    <t>Iie, tegami zya arimasen desita yo.</t>
+  </si>
+  <si>
+    <t>Was it a letter?</t>
+  </si>
+  <si>
+    <t>No, it was not a letter.</t>
+  </si>
+  <si>
+    <t>Kiree desu ka?</t>
+  </si>
+  <si>
+    <t>Iie, kiree zya ariamsen yo.</t>
+  </si>
+  <si>
+    <t>Is it pretty?</t>
+  </si>
+  <si>
+    <t>No, it is not pretty.</t>
+  </si>
+  <si>
+    <t>Iie, kaimasen desita yo.</t>
+  </si>
+  <si>
+    <t>No, I did not buy it.</t>
+  </si>
+  <si>
+    <t>Simasu ka?</t>
+  </si>
+  <si>
+    <t>Iie, simasen yo.</t>
+  </si>
+  <si>
+    <t>Will you do it?</t>
+  </si>
+  <si>
+    <t>No, I will not do it.</t>
+  </si>
+  <si>
+    <t>No, it was not interesting.</t>
+  </si>
+  <si>
+    <t>Denwa desu ka?</t>
+  </si>
+  <si>
+    <t>Iie, denwa zya arimasen yo.</t>
+  </si>
+  <si>
+    <t>Was it the telephone?</t>
+  </si>
+  <si>
+    <t>No, it was not the telephone.</t>
+  </si>
+  <si>
+    <t>No, it was not expensive.</t>
+  </si>
+  <si>
+    <t>Iie, yoku arimasen desu yo.</t>
+  </si>
+  <si>
+    <t>Iie, omosiroku arimasen desita yo.</t>
+  </si>
+  <si>
+    <t>Iie, takaku arimasen desu yo.</t>
+  </si>
+  <si>
+    <t>(Switch ne! with nee)
+Speaker A:</t>
+  </si>
+  <si>
+    <t>(Switch ne! with nee)
+Speaker B:</t>
+  </si>
+  <si>
+    <t>Kiree desu ne!</t>
+  </si>
+  <si>
+    <t>Soo desu ne! Kiree desu ne!</t>
+  </si>
+  <si>
+    <t>It's pretty, isn't it.</t>
+  </si>
+  <si>
+    <t>That's right. It is pretty, isn't it.</t>
+  </si>
+  <si>
+    <t>Kiree desu nee.</t>
+  </si>
+  <si>
+    <t>Soo desu nee. Kiree desu nee.</t>
+  </si>
+  <si>
+    <t>Iya, nihongo zya arimasen yo. Tyuugokugo desu.</t>
+  </si>
+  <si>
+    <t>Is it Japanese?</t>
+  </si>
+  <si>
+    <t>No, it is not Japanese. It is Chinese.</t>
+  </si>
+  <si>
+    <t>Yamamoto-san zya nai desu ka?</t>
+  </si>
+  <si>
+    <t>A, soo desu ne!</t>
+  </si>
+  <si>
+    <t>Isn't that Mr. Yamamoto?</t>
+  </si>
+  <si>
+    <t>Oh, it is, isn't it.</t>
+  </si>
+  <si>
+    <t>Soo desu nee. Amari kiree zya nai desu nee.</t>
+  </si>
+  <si>
+    <t>Aa, soo desu ka. Zannen desu nee.</t>
+  </si>
+  <si>
+    <t>Is she pretty?</t>
+  </si>
+  <si>
+    <t>Hmm (Hesitation). She is not very pretty, is she!</t>
+  </si>
+  <si>
+    <t>Oh really? That's too bad, isn't it!</t>
+  </si>
+  <si>
+    <t>Tookyoo desita ka?</t>
+  </si>
+  <si>
+    <t>Iya, Tookyoo zya arimasen desita.</t>
+  </si>
+  <si>
+    <t>Was it Tokyo?</t>
+  </si>
+  <si>
+    <t>No, it was not Tokyo.</t>
+  </si>
+  <si>
+    <t>It's pretty, isn't it!</t>
+  </si>
+  <si>
+    <t>Hmm. It is pretty, isn't it!</t>
+  </si>
+  <si>
+    <t>Komarimase ne!</t>
+  </si>
+  <si>
+    <t>Soo desu ne! Komarimasu ne!</t>
+  </si>
+  <si>
+    <t>It's worrisome, isn't it.</t>
+  </si>
+  <si>
+    <t>That's right. It is worrisome, isn't it.</t>
+  </si>
+  <si>
+    <t>Accept</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>Kinoo</t>
+  </si>
+  <si>
+    <t>Kyoo</t>
+  </si>
+  <si>
+    <t>Asita</t>
+  </si>
+  <si>
+    <t>*****</t>
+  </si>
+  <si>
+    <t>$$$$</t>
+  </si>
+  <si>
+    <t>Sept. __</t>
+  </si>
+  <si>
+    <t>Est. 2015</t>
+  </si>
+  <si>
+    <t>1989 (Amari atarasiku nai desu yo.)</t>
+  </si>
+  <si>
+    <t>1950 (Hurui desu yo.)</t>
+  </si>
+  <si>
+    <t>Ee, wakarimasita.</t>
+  </si>
+  <si>
+    <t>Yes, I understood.</t>
+  </si>
+  <si>
+    <t>Aa, soo desu nee.</t>
   </si>
 </sst>
 </file>
@@ -2901,7 +3207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3038,21 +3344,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3069,6 +3360,60 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3688,11 +4033,11 @@
         <v>32</v>
       </c>
       <c r="D1"/>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="59" t="s">
         <v>453</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
     </row>
     <row r="2" spans="1:7" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -5094,15 +5439,15 @@
   <sheetData>
     <row r="1" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="61" t="s">
         <v>491</v>
       </c>
-      <c r="C1" s="49"/>
+      <c r="C1" s="62"/>
       <c r="D1" s="11"/>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="61" t="s">
         <v>492</v>
       </c>
-      <c r="F1" s="50"/>
+      <c r="F1" s="63"/>
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -6316,7 +6661,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>569</v>
@@ -6328,13 +6673,13 @@
         <v>570</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>685</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>686</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>687</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>101</v>
@@ -6764,8 +7109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:C28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -6779,547 +7124,513 @@
       <c r="A1" s="10" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="68" t="s">
         <v>554</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="53" t="s">
-        <v>554</v>
-      </c>
-      <c r="E1" s="54"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="64" t="s">
         <v>645</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="55" t="s">
-        <v>645</v>
-      </c>
-      <c r="E2" s="56"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="64" t="s">
+        <v>690</v>
+      </c>
+      <c r="E2" s="65"/>
     </row>
     <row r="3" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="66" t="s">
         <v>649</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="51" t="s">
-        <v>649</v>
-      </c>
-      <c r="E3" s="52"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E3" s="67"/>
     </row>
     <row r="4" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>556</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="68" t="s">
         <v>646</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="53" t="s">
-        <v>646</v>
-      </c>
-      <c r="E4" s="54"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E4" s="69"/>
     </row>
     <row r="5" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="64" t="s">
         <v>528</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="55" t="s">
-        <v>528</v>
-      </c>
-      <c r="E5" s="56"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="65"/>
     </row>
     <row r="6" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="66" t="s">
         <v>650</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="51" t="s">
-        <v>650</v>
-      </c>
-      <c r="E6" s="52"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="66" t="s">
+        <v>693</v>
+      </c>
+      <c r="E6" s="67"/>
     </row>
     <row r="7" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>557</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="68" t="s">
         <v>647</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="53" t="s">
-        <v>647</v>
-      </c>
-      <c r="E7" s="54"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E7" s="69"/>
     </row>
     <row r="8" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="64" t="s">
         <v>652</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="55" t="s">
-        <v>652</v>
-      </c>
-      <c r="E8" s="56"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="64" t="s">
+        <v>694</v>
+      </c>
+      <c r="E8" s="65"/>
     </row>
     <row r="9" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="66" t="s">
         <v>651</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="51" t="s">
-        <v>651</v>
-      </c>
-      <c r="E9" s="52"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="66" t="s">
+        <v>442</v>
+      </c>
+      <c r="E9" s="67"/>
     </row>
     <row r="10" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>558</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="68" t="s">
         <v>648</v>
       </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="53" t="s">
-        <v>648</v>
-      </c>
-      <c r="E10" s="54"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E10" s="69"/>
     </row>
     <row r="11" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="64" t="s">
         <v>653</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="55" t="s">
-        <v>653</v>
-      </c>
-      <c r="E11" s="56"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="64" t="s">
+        <v>548</v>
+      </c>
+      <c r="E11" s="65"/>
     </row>
     <row r="12" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="66" t="s">
         <v>654</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="51" t="s">
-        <v>654</v>
-      </c>
-      <c r="E12" s="52"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="66" t="s">
+        <v>697</v>
+      </c>
+      <c r="E12" s="67"/>
     </row>
     <row r="13" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>559</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="68" t="s">
         <v>655</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="53" t="s">
-        <v>655</v>
-      </c>
-      <c r="E13" s="54"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E13" s="69"/>
     </row>
     <row r="14" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="64" t="s">
         <v>656</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="55" t="s">
-        <v>656</v>
-      </c>
-      <c r="E14" s="56"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="64" t="s">
+        <v>789</v>
+      </c>
+      <c r="E14" s="65"/>
     </row>
     <row r="15" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="66" t="s">
         <v>657</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="51" t="s">
-        <v>657</v>
-      </c>
-      <c r="E15" s="52"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="66" t="s">
+        <v>790</v>
+      </c>
+      <c r="E15" s="67"/>
     </row>
     <row r="16" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>560</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="68" t="s">
         <v>658</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="53" t="s">
-        <v>658</v>
-      </c>
-      <c r="E16" s="54"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E16" s="69"/>
     </row>
     <row r="17" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="55" t="s">
-        <v>679</v>
-      </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="55" t="s">
-        <v>679</v>
-      </c>
-      <c r="E17" s="56"/>
+      <c r="B17" s="64" t="s">
+        <v>677</v>
+      </c>
+      <c r="C17" s="65"/>
+      <c r="D17" s="64" t="s">
+        <v>791</v>
+      </c>
+      <c r="E17" s="65"/>
     </row>
     <row r="18" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="66" t="s">
         <v>659</v>
       </c>
-      <c r="C18" s="52"/>
-      <c r="D18" s="51" t="s">
-        <v>659</v>
-      </c>
-      <c r="E18" s="52"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="67"/>
     </row>
     <row r="19" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>561</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="68" t="s">
         <v>660</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="53" t="s">
-        <v>660</v>
-      </c>
-      <c r="E19" s="54"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E19" s="69"/>
     </row>
     <row r="20" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="64" t="s">
         <v>661</v>
       </c>
-      <c r="C20" s="56"/>
-      <c r="D20" s="55" t="s">
-        <v>661</v>
-      </c>
-      <c r="E20" s="56"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="65"/>
     </row>
     <row r="21" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="66" t="s">
         <v>662</v>
       </c>
-      <c r="C21" s="52"/>
-      <c r="D21" s="51" t="s">
-        <v>662</v>
-      </c>
-      <c r="E21" s="52"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="67"/>
     </row>
     <row r="22" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>562</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="68" t="s">
         <v>663</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="53" t="s">
-        <v>663</v>
-      </c>
-      <c r="E22" s="54"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E22" s="69"/>
     </row>
     <row r="23" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="64" t="s">
         <v>664</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="55" t="s">
-        <v>664</v>
-      </c>
-      <c r="E23" s="56"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="65"/>
     </row>
     <row r="24" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="66" t="s">
         <v>665</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="51" t="s">
-        <v>665</v>
-      </c>
-      <c r="E24" s="52"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="67"/>
     </row>
     <row r="25" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>563</v>
       </c>
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="68" t="s">
         <v>666</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="53" t="s">
-        <v>666</v>
-      </c>
-      <c r="E25" s="54"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E25" s="69"/>
     </row>
     <row r="26" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="55" t="s">
-        <v>690</v>
-      </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="55" t="s">
-        <v>667</v>
-      </c>
-      <c r="E26" s="56"/>
+      <c r="B26" s="64" t="s">
+        <v>688</v>
+      </c>
+      <c r="C26" s="65"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="65"/>
     </row>
     <row r="27" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="51" t="s">
-        <v>691</v>
-      </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="51" t="s">
-        <v>668</v>
-      </c>
-      <c r="E27" s="52"/>
+      <c r="B27" s="66" t="s">
+        <v>689</v>
+      </c>
+      <c r="C27" s="67"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="67"/>
     </row>
     <row r="28" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>564</v>
       </c>
-      <c r="B28" s="53" t="s">
-        <v>669</v>
-      </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="53" t="s">
-        <v>669</v>
-      </c>
-      <c r="E28" s="54"/>
+      <c r="B28" s="68" t="s">
+        <v>667</v>
+      </c>
+      <c r="C28" s="69"/>
+      <c r="D28" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E28" s="69"/>
     </row>
     <row r="29" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="55" t="s">
-        <v>670</v>
-      </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="55" t="s">
-        <v>670</v>
-      </c>
-      <c r="E29" s="56"/>
+      <c r="B29" s="64" t="s">
+        <v>668</v>
+      </c>
+      <c r="C29" s="65"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="65"/>
     </row>
     <row r="30" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="51" t="s">
-        <v>671</v>
-      </c>
-      <c r="C30" s="52"/>
-      <c r="D30" s="51" t="s">
-        <v>671</v>
-      </c>
-      <c r="E30" s="52"/>
+      <c r="B30" s="66" t="s">
+        <v>669</v>
+      </c>
+      <c r="C30" s="67"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="67"/>
     </row>
     <row r="31" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>565</v>
       </c>
-      <c r="B31" s="53" t="s">
-        <v>672</v>
-      </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="53" t="s">
-        <v>672</v>
-      </c>
-      <c r="E31" s="54"/>
+      <c r="B31" s="68" t="s">
+        <v>670</v>
+      </c>
+      <c r="C31" s="69"/>
+      <c r="D31" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E31" s="69"/>
     </row>
     <row r="32" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="55" t="s">
-        <v>680</v>
-      </c>
-      <c r="C32" s="56"/>
-      <c r="D32" s="55" t="s">
-        <v>680</v>
-      </c>
-      <c r="E32" s="56"/>
+      <c r="B32" s="64" t="s">
+        <v>678</v>
+      </c>
+      <c r="C32" s="65"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="65"/>
     </row>
     <row r="33" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="51" t="s">
-        <v>673</v>
-      </c>
-      <c r="C33" s="52"/>
-      <c r="D33" s="51" t="s">
-        <v>673</v>
-      </c>
-      <c r="E33" s="52"/>
+      <c r="B33" s="66" t="s">
+        <v>671</v>
+      </c>
+      <c r="C33" s="67"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="67"/>
     </row>
     <row r="34" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>566</v>
       </c>
-      <c r="B34" s="53" t="s">
-        <v>674</v>
-      </c>
-      <c r="C34" s="54"/>
-      <c r="D34" s="53" t="s">
-        <v>674</v>
-      </c>
-      <c r="E34" s="54"/>
+      <c r="B34" s="68" t="s">
+        <v>672</v>
+      </c>
+      <c r="C34" s="69"/>
+      <c r="D34" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E34" s="69"/>
     </row>
     <row r="35" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="55" t="s">
-        <v>681</v>
-      </c>
-      <c r="C35" s="56"/>
-      <c r="D35" s="55" t="s">
-        <v>681</v>
-      </c>
-      <c r="E35" s="56"/>
+      <c r="B35" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="C35" s="65"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="65"/>
     </row>
     <row r="36" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="51" t="s">
-        <v>675</v>
-      </c>
-      <c r="C36" s="52"/>
-      <c r="D36" s="51" t="s">
-        <v>675</v>
-      </c>
-      <c r="E36" s="52"/>
+      <c r="B36" s="66" t="s">
+        <v>673</v>
+      </c>
+      <c r="C36" s="67"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="67"/>
     </row>
     <row r="37" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>567</v>
       </c>
-      <c r="B37" s="53" t="s">
-        <v>676</v>
-      </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="53" t="s">
-        <v>676</v>
-      </c>
-      <c r="E37" s="54"/>
+      <c r="B37" s="68" t="s">
+        <v>674</v>
+      </c>
+      <c r="C37" s="69"/>
+      <c r="D37" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E37" s="69"/>
     </row>
     <row r="38" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="55" t="s">
-        <v>682</v>
-      </c>
-      <c r="C38" s="56"/>
-      <c r="D38" s="55" t="s">
-        <v>682</v>
-      </c>
-      <c r="E38" s="56"/>
+      <c r="B38" s="64" t="s">
+        <v>680</v>
+      </c>
+      <c r="C38" s="65"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="65"/>
     </row>
     <row r="39" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="55" t="s">
-        <v>683</v>
-      </c>
-      <c r="C39" s="56"/>
-      <c r="D39" s="55" t="s">
-        <v>683</v>
-      </c>
-      <c r="E39" s="56"/>
+      <c r="B39" s="64" t="s">
+        <v>681</v>
+      </c>
+      <c r="C39" s="65"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="65"/>
     </row>
     <row r="40" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>568</v>
       </c>
-      <c r="B40" s="53" t="s">
-        <v>677</v>
-      </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="53" t="s">
-        <v>677</v>
-      </c>
-      <c r="E40" s="54"/>
+      <c r="B40" s="68" t="s">
+        <v>675</v>
+      </c>
+      <c r="C40" s="69"/>
+      <c r="D40" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="E40" s="69"/>
     </row>
     <row r="41" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="55" t="s">
+      <c r="B41" s="64" t="s">
         <v>528</v>
       </c>
-      <c r="C41" s="56"/>
-      <c r="D41" s="55" t="s">
-        <v>528</v>
-      </c>
-      <c r="E41" s="56"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="65"/>
     </row>
     <row r="42" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="51" t="s">
-        <v>678</v>
-      </c>
-      <c r="C42" s="52"/>
-      <c r="D42" s="51" t="s">
-        <v>678</v>
-      </c>
-      <c r="E42" s="52"/>
+      <c r="B42" s="66" t="s">
+        <v>676</v>
+      </c>
+      <c r="C42" s="67"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="67"/>
     </row>
     <row r="43" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7381,48 +7692,36 @@
     <row r="100" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
@@ -7435,36 +7734,48 @@
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7703,8 +8014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -8001,8 +8312,12 @@
       <c r="A20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
+      <c r="B20" s="13" t="s">
+        <v>687</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>756</v>
+      </c>
       <c r="D20" s="13"/>
       <c r="E20" s="14"/>
     </row>
@@ -8010,8 +8325,12 @@
       <c r="A21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
+      <c r="B21" s="16" t="s">
+        <v>757</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>758</v>
+      </c>
       <c r="D21" s="16"/>
       <c r="E21" s="17"/>
     </row>
@@ -8036,8 +8355,12 @@
       <c r="A23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
+      <c r="B23" s="13" t="s">
+        <v>759</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>760</v>
+      </c>
       <c r="D23" s="13"/>
       <c r="E23" s="14"/>
     </row>
@@ -8045,8 +8368,12 @@
       <c r="A24" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
+      <c r="B24" s="16" t="s">
+        <v>761</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>762</v>
+      </c>
       <c r="D24" s="16"/>
       <c r="E24" s="17"/>
     </row>
@@ -8071,18 +8398,30 @@
       <c r="A26" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
+      <c r="B26" s="13" t="s">
+        <v>729</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>763</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>764</v>
+      </c>
       <c r="E26" s="14"/>
     </row>
     <row r="27" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
+      <c r="B27" s="16" t="s">
+        <v>765</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>766</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>767</v>
+      </c>
       <c r="E27" s="17"/>
     </row>
     <row r="28" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8106,8 +8445,12 @@
       <c r="A29" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
+      <c r="B29" s="13" t="s">
+        <v>768</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>769</v>
+      </c>
       <c r="D29" s="13"/>
       <c r="E29" s="14"/>
     </row>
@@ -8115,80 +8458,56 @@
       <c r="A30" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
+      <c r="B30" s="16" t="s">
+        <v>770</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>771</v>
+      </c>
       <c r="D30" s="16"/>
       <c r="E30" s="17"/>
     </row>
     <row r="31" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
     </row>
     <row r="32" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="14"/>
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
     </row>
     <row r="33" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="17"/>
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
     </row>
     <row r="34" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
     </row>
     <row r="35" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="14"/>
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
     </row>
     <row r="36" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="17"/>
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
     </row>
     <row r="37" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9458,6 +9777,1340 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E100"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" style="5" customWidth="1"/>
+    <col min="2" max="8" width="46.7109375" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>699</v>
+      </c>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
+    </row>
+    <row r="3" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>700</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>701</v>
+      </c>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+    </row>
+    <row r="4" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>626</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>702</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="51"/>
+    </row>
+    <row r="6" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>705</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>706</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47"/>
+    </row>
+    <row r="7" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>703</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>704</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="51"/>
+    </row>
+    <row r="9" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>707</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>708</v>
+      </c>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+    </row>
+    <row r="10" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>709</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>710</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="51"/>
+    </row>
+    <row r="12" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>711</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>712</v>
+      </c>
+      <c r="D12" s="46"/>
+      <c r="E12" s="47"/>
+    </row>
+    <row r="13" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>713</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>714</v>
+      </c>
+      <c r="D14" s="50"/>
+      <c r="E14" s="51"/>
+    </row>
+    <row r="15" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>715</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>716</v>
+      </c>
+      <c r="D15" s="46"/>
+      <c r="E15" s="47"/>
+    </row>
+    <row r="16" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>717</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>718</v>
+      </c>
+      <c r="D17" s="50"/>
+      <c r="E17" s="51"/>
+    </row>
+    <row r="18" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>719</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>720</v>
+      </c>
+      <c r="D18" s="46"/>
+      <c r="E18" s="47"/>
+    </row>
+    <row r="19" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>695</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>721</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>722</v>
+      </c>
+      <c r="D20" s="50"/>
+      <c r="E20" s="51"/>
+    </row>
+    <row r="21" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>723</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>724</v>
+      </c>
+      <c r="D21" s="46"/>
+      <c r="E21" s="47"/>
+    </row>
+    <row r="22" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>696</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>725</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>726</v>
+      </c>
+      <c r="D23" s="50"/>
+      <c r="E23" s="51"/>
+    </row>
+    <row r="24" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>727</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>728</v>
+      </c>
+      <c r="D24" s="46"/>
+      <c r="E24" s="47"/>
+    </row>
+    <row r="25" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E100"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" style="5" customWidth="1"/>
+    <col min="2" max="8" width="46.7109375" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>729</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
+    </row>
+    <row r="3" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>731</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>732</v>
+      </c>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+    </row>
+    <row r="4" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>733</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="51"/>
+    </row>
+    <row r="6" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>734</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47"/>
+    </row>
+    <row r="7" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>745</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="51"/>
+    </row>
+    <row r="9" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>370</v>
+      </c>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+    </row>
+    <row r="10" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>626</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>702</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="51"/>
+    </row>
+    <row r="12" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>705</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>706</v>
+      </c>
+      <c r="D12" s="46"/>
+      <c r="E12" s="47"/>
+    </row>
+    <row r="13" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>735</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>736</v>
+      </c>
+      <c r="D14" s="50"/>
+      <c r="E14" s="51"/>
+    </row>
+    <row r="15" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>737</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>738</v>
+      </c>
+      <c r="D15" s="46"/>
+      <c r="E15" s="47"/>
+    </row>
+    <row r="16" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>746</v>
+      </c>
+      <c r="D17" s="50"/>
+      <c r="E17" s="51"/>
+    </row>
+    <row r="18" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>739</v>
+      </c>
+      <c r="D18" s="46"/>
+      <c r="E18" s="47"/>
+    </row>
+    <row r="19" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>740</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>741</v>
+      </c>
+      <c r="D20" s="50"/>
+      <c r="E20" s="51"/>
+    </row>
+    <row r="21" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>742</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>743</v>
+      </c>
+      <c r="D21" s="46"/>
+      <c r="E21" s="47"/>
+    </row>
+    <row r="22" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>747</v>
+      </c>
+      <c r="D23" s="50"/>
+      <c r="E23" s="51"/>
+    </row>
+    <row r="24" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>744</v>
+      </c>
+      <c r="D24" s="46"/>
+      <c r="E24" s="47"/>
+    </row>
+    <row r="25" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" style="5" customWidth="1"/>
+    <col min="2" max="8" width="46.7109375" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>748</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>750</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>751</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>754</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>752</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>753</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>772</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>748</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>774</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>775</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="51"/>
+    </row>
+    <row r="6" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>776</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>777</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47"/>
+    </row>
+    <row r="7" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>748</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="51"/>
+    </row>
+    <row r="9" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="46"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+    </row>
+    <row r="10" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>748</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="51"/>
+    </row>
+    <row r="12" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="46"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="47"/>
+    </row>
+    <row r="13" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>748</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="51"/>
+    </row>
+    <row r="15" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="46"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="47"/>
+    </row>
+    <row r="16" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>748</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="51"/>
+    </row>
+    <row r="18" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="46"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="47"/>
+    </row>
+    <row r="19" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>748</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="51"/>
+    </row>
+    <row r="21" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="46"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="47"/>
+    </row>
+    <row r="22" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>748</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="50"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="51"/>
+    </row>
+    <row r="24" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="46"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="47"/>
+    </row>
+    <row r="25" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9509,10 +11162,10 @@
         <v>569</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>589</v>
@@ -9561,7 +11214,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C5" s="44" t="s">
         <v>569</v>
@@ -9573,13 +11226,13 @@
         <v>570</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>685</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>686</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>687</v>
       </c>
       <c r="I5" s="45" t="s">
         <v>101</v>
@@ -10005,7 +11658,453 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F100"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" style="5" customWidth="1"/>
+    <col min="2" max="8" width="46.7109375" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+    </row>
+    <row r="3" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="55"/>
+    </row>
+    <row r="4" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="53"/>
+    </row>
+    <row r="6" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="55"/>
+    </row>
+    <row r="7" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="53"/>
+    </row>
+    <row r="9" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="55"/>
+    </row>
+    <row r="10" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+    </row>
+    <row r="12" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="55"/>
+    </row>
+    <row r="13" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="53"/>
+    </row>
+    <row r="15" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="55"/>
+    </row>
+    <row r="16" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="53"/>
+    </row>
+    <row r="18" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="55"/>
+    </row>
+    <row r="19" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="53"/>
+    </row>
+    <row r="21" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="55"/>
+    </row>
+    <row r="22" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="53"/>
+    </row>
+    <row r="24" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="55"/>
+    </row>
+    <row r="25" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="53"/>
+    </row>
+    <row r="27" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="55"/>
+    </row>
+    <row r="28" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="58" t="s">
+        <v>783</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>786</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="4" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="33" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
@@ -13183,11 +15282,11 @@
         <v>32</v>
       </c>
       <c r="D1"/>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="59" t="s">
         <v>452</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
     </row>
     <row r="2" spans="1:7" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
Study Guide update 2 9-24
</commit_message>
<xml_diff>
--- a/StudyGuide.xlsx
+++ b/StudyGuide.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\JPNSE 0001\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="614" firstSheet="15" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="614" firstSheet="15" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="1A Verbals" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2244" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2254" uniqueCount="801">
   <si>
     <t>Imperfective
 Negative</t>
@@ -2659,9 +2659,6 @@
     <t>Asita kimasu ne?</t>
   </si>
   <si>
-    <t>Dekimasita. Doozo.</t>
-  </si>
-  <si>
     <t>Tyotto..</t>
   </si>
   <si>
@@ -2997,7 +2994,41 @@
     <t>Yes, I understood.</t>
   </si>
   <si>
-    <t>Aa, soo desu nee.</t>
+    <t>Is that so? That's too bad.</t>
+  </si>
+  <si>
+    <t>Aa, yasukatta desu ka?</t>
+  </si>
+  <si>
+    <t>Oh, it was cheap?</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Nomimasen ka?</t>
+  </si>
+  <si>
+    <t>Won't you drink some?</t>
+  </si>
+  <si>
+    <t>Question (Invitation)</t>
+  </si>
+  <si>
+    <t>Ee, yoku tukurimasu yo.
+Ee, maa.
+Iie, amari yoku tukurimasen yo.</t>
+  </si>
+  <si>
+    <t>Ee, asita kimasu yo.
+Iie, asita kimasen yo.</t>
+  </si>
+  <si>
+    <t>Yes, I am coming tomorrow.
+No, I am not coming tomorrow.</t>
+  </si>
+  <si>
+    <t>Ee, Dekimasita. Doozo.</t>
   </si>
 </sst>
 </file>
@@ -3398,12 +3429,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3414,6 +3439,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6661,7 +6692,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>569</v>
@@ -6673,13 +6704,13 @@
         <v>570</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>684</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>685</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>101</v>
@@ -7109,8 +7140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -7124,513 +7155,533 @@
       <c r="A1" s="10" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="66" t="s">
         <v>554</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E1" s="69"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="68" t="s">
         <v>645</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="64" t="s">
-        <v>690</v>
-      </c>
-      <c r="E2" s="65"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="68" t="s">
+        <v>689</v>
+      </c>
+      <c r="E2" s="69"/>
     </row>
     <row r="3" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="64" t="s">
         <v>649</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="66" t="s">
-        <v>691</v>
-      </c>
-      <c r="E3" s="67"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="64" t="s">
+        <v>690</v>
+      </c>
+      <c r="E3" s="65"/>
     </row>
     <row r="4" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>556</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="66" t="s">
         <v>646</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E4" s="69"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="68" t="s">
         <v>528</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="64" t="s">
+      <c r="C5" s="69"/>
+      <c r="D5" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="E5" s="65"/>
+      <c r="E5" s="69"/>
     </row>
     <row r="6" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="64" t="s">
         <v>650</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="66" t="s">
-        <v>693</v>
-      </c>
-      <c r="E6" s="67"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="64" t="s">
+        <v>692</v>
+      </c>
+      <c r="E6" s="65"/>
     </row>
     <row r="7" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>557</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="66" t="s">
         <v>647</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E7" s="69"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E7" s="67"/>
     </row>
     <row r="8" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="68" t="s">
         <v>652</v>
       </c>
-      <c r="C8" s="65"/>
-      <c r="D8" s="64" t="s">
-        <v>694</v>
-      </c>
-      <c r="E8" s="65"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="68" t="s">
+        <v>693</v>
+      </c>
+      <c r="E8" s="69"/>
     </row>
     <row r="9" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="64" t="s">
         <v>651</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="66" t="s">
+      <c r="C9" s="65"/>
+      <c r="D9" s="64" t="s">
         <v>442</v>
       </c>
-      <c r="E9" s="67"/>
+      <c r="E9" s="65"/>
     </row>
     <row r="10" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>558</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="66" t="s">
         <v>648</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E10" s="69"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E10" s="67"/>
     </row>
     <row r="11" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="68" t="s">
         <v>653</v>
       </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="64" t="s">
+      <c r="C11" s="69"/>
+      <c r="D11" s="68" t="s">
         <v>548</v>
       </c>
-      <c r="E11" s="65"/>
+      <c r="E11" s="69"/>
     </row>
     <row r="12" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="64" t="s">
         <v>654</v>
       </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="66" t="s">
-        <v>697</v>
-      </c>
-      <c r="E12" s="67"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="64" t="s">
+        <v>696</v>
+      </c>
+      <c r="E12" s="65"/>
     </row>
     <row r="13" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>559</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="66" t="s">
         <v>655</v>
       </c>
-      <c r="C13" s="69"/>
-      <c r="D13" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E13" s="69"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E13" s="67"/>
     </row>
     <row r="14" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="68" t="s">
         <v>656</v>
       </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="64" t="s">
-        <v>789</v>
-      </c>
-      <c r="E14" s="65"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="68" t="s">
+        <v>788</v>
+      </c>
+      <c r="E14" s="69"/>
     </row>
     <row r="15" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="64" t="s">
         <v>657</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="66" t="s">
-        <v>790</v>
-      </c>
-      <c r="E15" s="67"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="64" t="s">
+        <v>789</v>
+      </c>
+      <c r="E15" s="65"/>
     </row>
     <row r="16" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>560</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="66" t="s">
         <v>658</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E16" s="69"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E16" s="67"/>
     </row>
     <row r="17" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="68" t="s">
         <v>677</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="64" t="s">
-        <v>791</v>
-      </c>
-      <c r="E17" s="65"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="68" t="s">
+        <v>763</v>
+      </c>
+      <c r="E17" s="69"/>
     </row>
     <row r="18" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="64" t="s">
         <v>659</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="67"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="64" t="s">
+        <v>790</v>
+      </c>
+      <c r="E18" s="65"/>
     </row>
     <row r="19" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>561</v>
       </c>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="66" t="s">
         <v>660</v>
       </c>
-      <c r="C19" s="69"/>
-      <c r="D19" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E19" s="69"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E19" s="67"/>
     </row>
     <row r="20" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="68" t="s">
         <v>661</v>
       </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="65"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="68" t="s">
+        <v>791</v>
+      </c>
+      <c r="E20" s="69"/>
     </row>
     <row r="21" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="64" t="s">
         <v>662</v>
       </c>
-      <c r="C21" s="67"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="67"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="64" t="s">
+        <v>792</v>
+      </c>
+      <c r="E21" s="65"/>
     </row>
     <row r="22" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>562</v>
       </c>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="66" t="s">
         <v>663</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E22" s="69"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="66" t="s">
+        <v>796</v>
+      </c>
+      <c r="E22" s="67"/>
     </row>
     <row r="23" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="68" t="s">
         <v>664</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="65"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="68" t="s">
+        <v>794</v>
+      </c>
+      <c r="E23" s="69"/>
     </row>
     <row r="24" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="64" t="s">
         <v>665</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="67"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="64" t="s">
+        <v>795</v>
+      </c>
+      <c r="E24" s="65"/>
     </row>
     <row r="25" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>563</v>
       </c>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="66" t="s">
         <v>666</v>
       </c>
-      <c r="C25" s="69"/>
-      <c r="D25" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E25" s="69"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E25" s="67"/>
     </row>
     <row r="26" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="64" t="s">
-        <v>688</v>
-      </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="65"/>
+      <c r="B26" s="68" t="s">
+        <v>687</v>
+      </c>
+      <c r="C26" s="69"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="69"/>
     </row>
     <row r="27" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="66" t="s">
-        <v>689</v>
-      </c>
-      <c r="C27" s="67"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="67"/>
+      <c r="B27" s="64" t="s">
+        <v>688</v>
+      </c>
+      <c r="C27" s="65"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="65"/>
     </row>
     <row r="28" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>564</v>
       </c>
-      <c r="B28" s="68" t="s">
+      <c r="B28" s="66" t="s">
         <v>667</v>
       </c>
-      <c r="C28" s="69"/>
-      <c r="D28" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E28" s="69"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E28" s="67"/>
     </row>
     <row r="29" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="68" t="s">
         <v>668</v>
       </c>
-      <c r="C29" s="65"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="65"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="68" t="s">
+        <v>797</v>
+      </c>
+      <c r="E29" s="69"/>
     </row>
     <row r="30" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="64" t="s">
         <v>669</v>
       </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="67"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="65"/>
     </row>
     <row r="31" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>565</v>
       </c>
-      <c r="B31" s="68" t="s">
+      <c r="B31" s="66" t="s">
         <v>670</v>
       </c>
-      <c r="C31" s="69"/>
-      <c r="D31" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E31" s="69"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E31" s="67"/>
     </row>
     <row r="32" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="64" t="s">
+      <c r="B32" s="68" t="s">
         <v>678</v>
       </c>
-      <c r="C32" s="65"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="65"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="68" t="s">
+        <v>798</v>
+      </c>
+      <c r="E32" s="69"/>
     </row>
     <row r="33" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="66" t="s">
+      <c r="B33" s="64" t="s">
         <v>671</v>
       </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="67"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="64" t="s">
+        <v>799</v>
+      </c>
+      <c r="E33" s="65"/>
     </row>
     <row r="34" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>566</v>
       </c>
-      <c r="B34" s="68" t="s">
+      <c r="B34" s="66" t="s">
         <v>672</v>
       </c>
-      <c r="C34" s="69"/>
-      <c r="D34" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E34" s="69"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="66" t="s">
+        <v>793</v>
+      </c>
+      <c r="E34" s="67"/>
     </row>
     <row r="35" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="64" t="s">
-        <v>679</v>
-      </c>
-      <c r="C35" s="65"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="65"/>
+      <c r="B35" s="68" t="s">
+        <v>800</v>
+      </c>
+      <c r="C35" s="69"/>
+      <c r="D35" s="68" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" s="69"/>
     </row>
     <row r="36" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="66" t="s">
+      <c r="B36" s="64" t="s">
         <v>673</v>
       </c>
-      <c r="C36" s="67"/>
-      <c r="D36" s="66"/>
-      <c r="E36" s="67"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="64" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="65"/>
     </row>
     <row r="37" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>567</v>
       </c>
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="66" t="s">
         <v>674</v>
       </c>
-      <c r="C37" s="69"/>
-      <c r="D37" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E37" s="69"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E37" s="67"/>
     </row>
     <row r="38" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="64" t="s">
-        <v>680</v>
-      </c>
-      <c r="C38" s="65"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="65"/>
+      <c r="B38" s="68" t="s">
+        <v>679</v>
+      </c>
+      <c r="C38" s="69"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="69"/>
     </row>
     <row r="39" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="64" t="s">
-        <v>681</v>
-      </c>
-      <c r="C39" s="65"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="65"/>
+      <c r="B39" s="68" t="s">
+        <v>680</v>
+      </c>
+      <c r="C39" s="69"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="69"/>
     </row>
     <row r="40" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>568</v>
       </c>
-      <c r="B40" s="68" t="s">
+      <c r="B40" s="66" t="s">
         <v>675</v>
       </c>
-      <c r="C40" s="69"/>
-      <c r="D40" s="68" t="s">
-        <v>692</v>
-      </c>
-      <c r="E40" s="69"/>
+      <c r="C40" s="67"/>
+      <c r="D40" s="66" t="s">
+        <v>691</v>
+      </c>
+      <c r="E40" s="67"/>
     </row>
     <row r="41" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="64" t="s">
+      <c r="B41" s="68" t="s">
         <v>528</v>
       </c>
-      <c r="C41" s="65"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="65"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="69"/>
     </row>
     <row r="42" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="66" t="s">
+      <c r="B42" s="64" t="s">
         <v>676</v>
       </c>
-      <c r="C42" s="67"/>
-      <c r="D42" s="66"/>
-      <c r="E42" s="67"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="65"/>
     </row>
     <row r="43" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7692,12 +7743,72 @@
     <row r="100" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
@@ -7710,72 +7821,12 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8313,10 +8364,10 @@
         <v>33</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="14"/>
@@ -8326,10 +8377,10 @@
         <v>34</v>
       </c>
       <c r="B21" s="16" t="s">
+        <v>756</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>757</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>758</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="17"/>
@@ -8356,10 +8407,10 @@
         <v>33</v>
       </c>
       <c r="B23" s="13" t="s">
+        <v>758</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>759</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>760</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="14"/>
@@ -8369,10 +8420,10 @@
         <v>34</v>
       </c>
       <c r="B24" s="16" t="s">
+        <v>760</v>
+      </c>
+      <c r="C24" s="16" t="s">
         <v>761</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>762</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="17"/>
@@ -8399,13 +8450,13 @@
         <v>33</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C26" s="13" t="s">
+        <v>762</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>763</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>764</v>
       </c>
       <c r="E26" s="14"/>
     </row>
@@ -8414,13 +8465,13 @@
         <v>34</v>
       </c>
       <c r="B27" s="16" t="s">
+        <v>764</v>
+      </c>
+      <c r="C27" s="16" t="s">
         <v>765</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="D27" s="16" t="s">
         <v>766</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>767</v>
       </c>
       <c r="E27" s="17"/>
     </row>
@@ -8446,10 +8497,10 @@
         <v>33</v>
       </c>
       <c r="B29" s="13" t="s">
+        <v>767</v>
+      </c>
+      <c r="C29" s="13" t="s">
         <v>768</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>769</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="14"/>
@@ -8459,10 +8510,10 @@
         <v>34</v>
       </c>
       <c r="B30" s="16" t="s">
+        <v>769</v>
+      </c>
+      <c r="C30" s="16" t="s">
         <v>770</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>771</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="17"/>
@@ -9812,10 +9863,10 @@
         <v>33</v>
       </c>
       <c r="B2" s="50" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2" s="50" t="s">
         <v>698</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>699</v>
       </c>
       <c r="D2" s="50"/>
       <c r="E2" s="51"/>
@@ -9825,10 +9876,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="46" t="s">
+        <v>699</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>700</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>701</v>
       </c>
       <c r="D3" s="46"/>
       <c r="E3" s="47"/>
@@ -9858,7 +9909,7 @@
         <v>626</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="51"/>
@@ -9868,10 +9919,10 @@
         <v>34</v>
       </c>
       <c r="B6" s="46" t="s">
+        <v>704</v>
+      </c>
+      <c r="C6" s="46" t="s">
         <v>705</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>706</v>
       </c>
       <c r="D6" s="46"/>
       <c r="E6" s="47"/>
@@ -9898,10 +9949,10 @@
         <v>33</v>
       </c>
       <c r="B8" s="50" t="s">
+        <v>702</v>
+      </c>
+      <c r="C8" s="50" t="s">
         <v>703</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>704</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="51"/>
@@ -9911,10 +9962,10 @@
         <v>34</v>
       </c>
       <c r="B9" s="46" t="s">
+        <v>706</v>
+      </c>
+      <c r="C9" s="46" t="s">
         <v>707</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>708</v>
       </c>
       <c r="D9" s="46"/>
       <c r="E9" s="47"/>
@@ -9941,10 +9992,10 @@
         <v>33</v>
       </c>
       <c r="B11" s="50" t="s">
+        <v>708</v>
+      </c>
+      <c r="C11" s="50" t="s">
         <v>709</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>710</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="51"/>
@@ -9954,10 +10005,10 @@
         <v>34</v>
       </c>
       <c r="B12" s="46" t="s">
+        <v>710</v>
+      </c>
+      <c r="C12" s="46" t="s">
         <v>711</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>712</v>
       </c>
       <c r="D12" s="46"/>
       <c r="E12" s="47"/>
@@ -9984,10 +10035,10 @@
         <v>33</v>
       </c>
       <c r="B14" s="50" t="s">
+        <v>712</v>
+      </c>
+      <c r="C14" s="50" t="s">
         <v>713</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>714</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="51"/>
@@ -9997,10 +10048,10 @@
         <v>34</v>
       </c>
       <c r="B15" s="46" t="s">
+        <v>714</v>
+      </c>
+      <c r="C15" s="46" t="s">
         <v>715</v>
-      </c>
-      <c r="C15" s="46" t="s">
-        <v>716</v>
       </c>
       <c r="D15" s="46"/>
       <c r="E15" s="47"/>
@@ -10027,10 +10078,10 @@
         <v>33</v>
       </c>
       <c r="B17" s="50" t="s">
+        <v>716</v>
+      </c>
+      <c r="C17" s="50" t="s">
         <v>717</v>
-      </c>
-      <c r="C17" s="50" t="s">
-        <v>718</v>
       </c>
       <c r="D17" s="50"/>
       <c r="E17" s="51"/>
@@ -10040,17 +10091,17 @@
         <v>34</v>
       </c>
       <c r="B18" s="46" t="s">
+        <v>718</v>
+      </c>
+      <c r="C18" s="46" t="s">
         <v>719</v>
-      </c>
-      <c r="C18" s="46" t="s">
-        <v>720</v>
       </c>
       <c r="D18" s="46"/>
       <c r="E18" s="47"/>
     </row>
     <row r="19" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B19" s="48" t="s">
         <v>31</v>
@@ -10070,10 +10121,10 @@
         <v>33</v>
       </c>
       <c r="B20" s="50" t="s">
+        <v>720</v>
+      </c>
+      <c r="C20" s="50" t="s">
         <v>721</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>722</v>
       </c>
       <c r="D20" s="50"/>
       <c r="E20" s="51"/>
@@ -10083,17 +10134,17 @@
         <v>34</v>
       </c>
       <c r="B21" s="46" t="s">
+        <v>722</v>
+      </c>
+      <c r="C21" s="46" t="s">
         <v>723</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>724</v>
       </c>
       <c r="D21" s="46"/>
       <c r="E21" s="47"/>
     </row>
     <row r="22" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B22" s="48" t="s">
         <v>31</v>
@@ -10113,10 +10164,10 @@
         <v>33</v>
       </c>
       <c r="B23" s="50" t="s">
+        <v>724</v>
+      </c>
+      <c r="C23" s="50" t="s">
         <v>725</v>
-      </c>
-      <c r="C23" s="50" t="s">
-        <v>726</v>
       </c>
       <c r="D23" s="50"/>
       <c r="E23" s="51"/>
@@ -10126,10 +10177,10 @@
         <v>34</v>
       </c>
       <c r="B24" s="46" t="s">
+        <v>726</v>
+      </c>
+      <c r="C24" s="46" t="s">
         <v>727</v>
-      </c>
-      <c r="C24" s="46" t="s">
-        <v>728</v>
       </c>
       <c r="D24" s="46"/>
       <c r="E24" s="47"/>
@@ -10270,10 +10321,10 @@
         <v>33</v>
       </c>
       <c r="B2" s="50" t="s">
+        <v>728</v>
+      </c>
+      <c r="C2" s="50" t="s">
         <v>729</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>730</v>
       </c>
       <c r="D2" s="50"/>
       <c r="E2" s="51"/>
@@ -10283,10 +10334,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="46" t="s">
+        <v>730</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>731</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>732</v>
       </c>
       <c r="D3" s="46"/>
       <c r="E3" s="47"/>
@@ -10316,7 +10367,7 @@
         <v>130</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="51"/>
@@ -10329,7 +10380,7 @@
         <v>139</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D6" s="46"/>
       <c r="E6" s="47"/>
@@ -10359,7 +10410,7 @@
         <v>109</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="51"/>
@@ -10402,7 +10453,7 @@
         <v>626</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="51"/>
@@ -10412,10 +10463,10 @@
         <v>34</v>
       </c>
       <c r="B12" s="46" t="s">
+        <v>704</v>
+      </c>
+      <c r="C12" s="46" t="s">
         <v>705</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>706</v>
       </c>
       <c r="D12" s="46"/>
       <c r="E12" s="47"/>
@@ -10442,10 +10493,10 @@
         <v>33</v>
       </c>
       <c r="B14" s="50" t="s">
+        <v>734</v>
+      </c>
+      <c r="C14" s="50" t="s">
         <v>735</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>736</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="51"/>
@@ -10455,10 +10506,10 @@
         <v>34</v>
       </c>
       <c r="B15" s="46" t="s">
+        <v>736</v>
+      </c>
+      <c r="C15" s="46" t="s">
         <v>737</v>
-      </c>
-      <c r="C15" s="46" t="s">
-        <v>738</v>
       </c>
       <c r="D15" s="46"/>
       <c r="E15" s="47"/>
@@ -10488,7 +10539,7 @@
         <v>269</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D17" s="50"/>
       <c r="E17" s="51"/>
@@ -10501,7 +10552,7 @@
         <v>137</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D18" s="46"/>
       <c r="E18" s="47"/>
@@ -10528,10 +10579,10 @@
         <v>33</v>
       </c>
       <c r="B20" s="50" t="s">
+        <v>739</v>
+      </c>
+      <c r="C20" s="50" t="s">
         <v>740</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>741</v>
       </c>
       <c r="D20" s="50"/>
       <c r="E20" s="51"/>
@@ -10541,10 +10592,10 @@
         <v>34</v>
       </c>
       <c r="B21" s="46" t="s">
+        <v>741</v>
+      </c>
+      <c r="C21" s="46" t="s">
         <v>742</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>743</v>
       </c>
       <c r="D21" s="46"/>
       <c r="E21" s="47"/>
@@ -10574,7 +10625,7 @@
         <v>147</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D23" s="50"/>
       <c r="E23" s="51"/>
@@ -10587,7 +10638,7 @@
         <v>149</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D24" s="46"/>
       <c r="E24" s="47"/>
@@ -10717,10 +10768,10 @@
         <v>32</v>
       </c>
       <c r="D1" s="48" t="s">
+        <v>747</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>748</v>
-      </c>
-      <c r="E1" s="49" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10728,16 +10779,16 @@
         <v>33</v>
       </c>
       <c r="B2" s="50" t="s">
+        <v>749</v>
+      </c>
+      <c r="C2" s="51" t="s">
         <v>750</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>751</v>
-      </c>
       <c r="D2" s="50" t="s">
+        <v>753</v>
+      </c>
+      <c r="E2" s="51" t="s">
         <v>754</v>
-      </c>
-      <c r="E2" s="51" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10745,16 +10796,16 @@
         <v>34</v>
       </c>
       <c r="B3" s="46" t="s">
+        <v>751</v>
+      </c>
+      <c r="C3" s="47" t="s">
         <v>752</v>
       </c>
-      <c r="C3" s="47" t="s">
-        <v>753</v>
-      </c>
       <c r="D3" s="46" t="s">
+        <v>771</v>
+      </c>
+      <c r="E3" s="47" t="s">
         <v>772</v>
-      </c>
-      <c r="E3" s="47" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10768,10 +10819,10 @@
         <v>32</v>
       </c>
       <c r="D4" s="48" t="s">
+        <v>747</v>
+      </c>
+      <c r="E4" s="49" t="s">
         <v>748</v>
-      </c>
-      <c r="E4" s="49" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10779,10 +10830,10 @@
         <v>33</v>
       </c>
       <c r="B5" s="50" t="s">
+        <v>773</v>
+      </c>
+      <c r="C5" s="51" t="s">
         <v>774</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>775</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="51"/>
@@ -10792,10 +10843,10 @@
         <v>34</v>
       </c>
       <c r="B6" s="46" t="s">
+        <v>775</v>
+      </c>
+      <c r="C6" s="47" t="s">
         <v>776</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>777</v>
       </c>
       <c r="D6" s="46"/>
       <c r="E6" s="47"/>
@@ -10811,10 +10862,10 @@
         <v>32</v>
       </c>
       <c r="D7" s="48" t="s">
+        <v>747</v>
+      </c>
+      <c r="E7" s="49" t="s">
         <v>748</v>
-      </c>
-      <c r="E7" s="49" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10846,10 +10897,10 @@
         <v>32</v>
       </c>
       <c r="D10" s="48" t="s">
+        <v>747</v>
+      </c>
+      <c r="E10" s="49" t="s">
         <v>748</v>
-      </c>
-      <c r="E10" s="49" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10881,10 +10932,10 @@
         <v>32</v>
       </c>
       <c r="D13" s="48" t="s">
+        <v>747</v>
+      </c>
+      <c r="E13" s="49" t="s">
         <v>748</v>
-      </c>
-      <c r="E13" s="49" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10916,10 +10967,10 @@
         <v>32</v>
       </c>
       <c r="D16" s="48" t="s">
+        <v>747</v>
+      </c>
+      <c r="E16" s="49" t="s">
         <v>748</v>
-      </c>
-      <c r="E16" s="49" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10951,10 +11002,10 @@
         <v>32</v>
       </c>
       <c r="D19" s="48" t="s">
+        <v>747</v>
+      </c>
+      <c r="E19" s="49" t="s">
         <v>748</v>
-      </c>
-      <c r="E19" s="49" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10986,10 +11037,10 @@
         <v>32</v>
       </c>
       <c r="D22" s="48" t="s">
+        <v>747</v>
+      </c>
+      <c r="E22" s="49" t="s">
         <v>748</v>
-      </c>
-      <c r="E22" s="49" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11162,10 +11213,10 @@
         <v>569</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>589</v>
@@ -11214,7 +11265,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C5" s="44" t="s">
         <v>569</v>
@@ -11226,13 +11277,13 @@
         <v>570</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>684</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>685</v>
       </c>
       <c r="I5" s="45" t="s">
         <v>101</v>
@@ -11990,45 +12041,45 @@
     </row>
     <row r="28" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
+        <v>779</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>780</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>781</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="58" t="s">
+        <v>782</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>783</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>784</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>785</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>786</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F32" s="4" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="33" ht="77.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>